<commit_message>
start gui; imrpove order management
</commit_message>
<xml_diff>
--- a/source/EliteQuant/Brokers/state_change.xlsx
+++ b/source/EliteQuant/Brokers/state_change.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="75">
   <si>
     <t>brokerage_client</t>
   </si>
@@ -234,6 +234,18 @@
   </si>
   <si>
     <t>ReqQryInstrument</t>
+  </si>
+  <si>
+    <t>ReqQryTradingAccount</t>
+  </si>
+  <si>
+    <t>OnRspQryTradingAccount</t>
+  </si>
+  <si>
+    <t>ReqQryInvestorPosition</t>
+  </si>
+  <si>
+    <t>onRspQryInvestorPosition</t>
   </si>
 </sst>
 </file>
@@ -1077,10 +1089,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,135 +1230,135 @@
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="C13" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="D14" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="9" t="s">
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="4" t="s">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E27" s="6"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="B28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>61</v>
-      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="6"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="A29" s="5"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="C29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="B30" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="6"/>
+      <c r="D30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
+      <c r="A31" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="B31" s="1"/>
-      <c r="C31" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E31" s="6"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="16" t="s">
-        <v>54</v>
+      <c r="B32" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1354,35 +1366,55 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="D33" s="1" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="E33" s="6"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="B34" s="1" t="s">
-        <v>29</v>
+      <c r="B34" s="16" t="s">
+        <v>54</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="B36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
-      <c r="B35" s="8" t="s">
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="9"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="1"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="9"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>